<commit_message>
upd account and IELTS words
</commit_message>
<xml_diff>
--- a/personal space(program)/accountBook2024.xlsx
+++ b/personal space(program)/accountBook2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hzhu41/myself/personGit/zhubiye/personal space(program)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7005996A-6202-D94A-A4C0-8055259355C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF42275E-61EA-BE48-95CC-6493A5BD3B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16800" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8520" yWindow="740" windowWidth="20880" windowHeight="18380" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024.01" sheetId="1" r:id="rId1"/>
@@ -249,61 +249,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -486,55 +431,110 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1788,24 +1788,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{67D8F19C-2DD0-4C59-A51B-15F75423EB7C}" name="表2_4561012" displayName="表2_4561012" ref="A1:N33" totalsRowCount="1" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="A1:N32" xr:uid="{4783F111-60E6-47B5-9AB1-437C496BFA64}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{C618F720-E758-4091-95B9-A16A4EBA1533}" name="日期" dataDxfId="69" totalsRowDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{1F96E219-DB50-486F-8570-DBF44B38E22B}" name="吃饭" dataDxfId="68" totalsRowDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{61EAFF41-5888-489B-9196-DD786161C5A4}" name="馋" dataDxfId="67" totalsRowDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{6E99EAD5-EE3A-451E-A248-40CBED41332E}" name="小余" dataDxfId="66" totalsRowDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{18C21F06-9B37-4402-892B-FCA37741E227}" name="生活" dataDxfId="65" totalsRowDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{80AB4C13-A583-4A87-AD6C-EBEB3448A8FA}" name="交通" dataDxfId="64" totalsRowDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{FEDAECBF-1E5D-42BF-8136-D0FBD99DC3D5}" name="爱好" dataDxfId="63" totalsRowDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{14F9E726-25B5-46A2-96B9-D5992FA69E71}" name="房租" dataDxfId="62" totalsRowDxfId="20">
+    <tableColumn id="1" xr3:uid="{C618F720-E758-4091-95B9-A16A4EBA1533}" name="日期" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{1F96E219-DB50-486F-8570-DBF44B38E22B}" name="吃饭" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{61EAFF41-5888-489B-9196-DD786161C5A4}" name="馋" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{6E99EAD5-EE3A-451E-A248-40CBED41332E}" name="小余" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{18C21F06-9B37-4402-892B-FCA37741E227}" name="生活" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="15" xr3:uid="{80AB4C13-A583-4A87-AD6C-EBEB3448A8FA}" name="交通" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{FEDAECBF-1E5D-42BF-8136-D0FBD99DC3D5}" name="爱好" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{14F9E726-25B5-46A2-96B9-D5992FA69E71}" name="房租" dataDxfId="55" totalsRowDxfId="54">
       <calculatedColumnFormula>2700/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{63C1CCED-5794-4D08-8697-AB2B01E7754E}" name="水电话费" dataDxfId="61" totalsRowDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{6E91D01F-56E9-4E7F-B53D-3D3FF4A281E3}" name="懒" dataDxfId="60" totalsRowDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{8852A42C-B4B0-429A-9AE4-B9BF56FE665D}" name="玩" dataDxfId="59" totalsRowDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{C1BD7762-6CD1-4FD0-8EBD-97061B85B0B0}" name="学习阅读" totalsRowFunction="custom" dataDxfId="58" totalsRowDxfId="16">
+    <tableColumn id="8" xr3:uid="{63C1CCED-5794-4D08-8697-AB2B01E7754E}" name="水电话费" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{6E91D01F-56E9-4E7F-B53D-3D3FF4A281E3}" name="懒" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="11" xr3:uid="{8852A42C-B4B0-429A-9AE4-B9BF56FE665D}" name="玩" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{C1BD7762-6CD1-4FD0-8EBD-97061B85B0B0}" name="学习阅读" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="46">
       <totalsRowFormula>SUM(B32:L32)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{50DF8B32-D09B-4C54-A088-827A73BFB4FC}" name="合计" dataDxfId="57" totalsRowDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{6E500027-168E-49B0-AD9B-D8F1510ABA55}" name="合计（）" dataDxfId="56" totalsRowDxfId="14">
+    <tableColumn id="13" xr3:uid="{50DF8B32-D09B-4C54-A088-827A73BFB4FC}" name="合计" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{6E500027-168E-49B0-AD9B-D8F1510ABA55}" name="合计（）" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula>表2_4561012[[#This Row],[合计]]-表2_4561012[[#This Row],[房租]]-表2_4561012[[#This Row],[水电话费]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1814,25 +1814,25 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{645319BD-A988-5446-B903-1527987D9691}" name="表2_47891113" displayName="表2_47891113" ref="A1:N34" totalsRowCount="1" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{645319BD-A988-5446-B903-1527987D9691}" name="表2_47891113" displayName="表2_47891113" ref="A1:N34" totalsRowCount="1" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:N33" xr:uid="{6C7D2DC4-9681-4990-8C7D-41F70811D8BA}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{EA524901-D4EC-A143-A509-4FD275E97CC6}" name="日期" dataDxfId="53" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{C06497D2-2A0D-2649-827A-35C6E82D9D91}" name="吃饭" dataDxfId="52" totalsRowDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{6A7BC9E3-719C-F348-AB4E-BB0E02ADE237}" name="馋" dataDxfId="51" totalsRowDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{F137B229-6D97-B64D-9BF5-8326E14B5C8B}" name="小余" dataDxfId="50" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{198A7588-A5CE-5E4A-A0BF-6145E223EB5D}" name="生活" dataDxfId="49" totalsRowDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{56B8C983-13AB-9B4E-9E7C-6C4D07E6B38D}" name="交通" dataDxfId="48" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{B58B3E08-229C-A445-8F80-C55776604CC5}" name="爱好" dataDxfId="47" totalsRowDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{38F24E93-E9B0-EB4F-B366-FB004F9495B5}" name="房租" dataDxfId="46" totalsRowDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{847F5526-E01C-B84B-8D3E-EB2FA614CB52}" name="水电话费" dataDxfId="45" totalsRowDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{5488EA85-2373-B948-9F06-8611ADD0094D}" name="懒" dataDxfId="44" totalsRowDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{E48F9FAC-A487-E045-8C67-B5BA7561B072}" name="玩" dataDxfId="43" totalsRowDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{98778E7E-4066-4942-ABC3-316D523FDD18}" name="学习阅读" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="2">
+    <tableColumn id="1" xr3:uid="{EA524901-D4EC-A143-A509-4FD275E97CC6}" name="日期" dataDxfId="39" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{C06497D2-2A0D-2649-827A-35C6E82D9D91}" name="吃饭" dataDxfId="38" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{6A7BC9E3-719C-F348-AB4E-BB0E02ADE237}" name="馋" dataDxfId="37" totalsRowDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{F137B229-6D97-B64D-9BF5-8326E14B5C8B}" name="小余" dataDxfId="36" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{198A7588-A5CE-5E4A-A0BF-6145E223EB5D}" name="生活" dataDxfId="35" totalsRowDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{56B8C983-13AB-9B4E-9E7C-6C4D07E6B38D}" name="交通" dataDxfId="34" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{B58B3E08-229C-A445-8F80-C55776604CC5}" name="爱好" dataDxfId="33" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{38F24E93-E9B0-EB4F-B366-FB004F9495B5}" name="房租" dataDxfId="32" totalsRowDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{847F5526-E01C-B84B-8D3E-EB2FA614CB52}" name="水电话费" dataDxfId="31" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{5488EA85-2373-B948-9F06-8611ADD0094D}" name="懒" dataDxfId="30" totalsRowDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{E48F9FAC-A487-E045-8C67-B5BA7561B072}" name="玩" dataDxfId="29" totalsRowDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{98778E7E-4066-4942-ABC3-316D523FDD18}" name="学习阅读" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="2">
       <totalsRowFormula>SUM(B33:L33)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{E0C49954-4FF8-984C-B61C-B7A706A680F7}" name="合计" dataDxfId="41" totalsRowDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{34F0172F-AFB8-5846-9873-F3D4B9DE1127}" name="合计（）" dataDxfId="40" totalsRowDxfId="0">
+    <tableColumn id="13" xr3:uid="{E0C49954-4FF8-984C-B61C-B7A706A680F7}" name="合计" dataDxfId="27" totalsRowDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{34F0172F-AFB8-5846-9873-F3D4B9DE1127}" name="合计（）" dataDxfId="26" totalsRowDxfId="0">
       <calculatedColumnFormula>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3421,7 +3421,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N32">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4512,7 +4512,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N32">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5598,7 +5598,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5614,8 +5614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D443F6-5FD4-C040-9D36-5DB36F99215C}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="151" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5881,7 +5881,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -5896,22 +5896,31 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3">
         <f>SUM(表2_47891113[[#This Row],[吃饭]:[学习阅读]])</f>
-        <v>84.38</v>
+        <v>94.38</v>
       </c>
       <c r="N8" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>39.379999999999995</v>
+        <v>49.379999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>45634</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="D9" s="3">
+        <f>15.74+29.5</f>
+        <v>45.24</v>
+      </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <v>9</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
@@ -5923,20 +5932,25 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3">
         <f>SUM(表2_47891113[[#This Row],[吃饭]:[学习阅读]])</f>
-        <v>45</v>
+        <v>125.64</v>
       </c>
       <c r="N9" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>0</v>
+        <v>80.64</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>45635</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <f>4.25+15.75</f>
+        <v>20</v>
+      </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3">
+        <v>79</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -5950,18 +5964,21 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3">
         <f>SUM(表2_47891113[[#This Row],[吃饭]:[学习阅读]])</f>
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="N10" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>45636</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <f>3.9+173.8+26.34</f>
+        <v>204.04000000000002</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -5977,19 +5994,23 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3">
         <f>SUM(表2_47891113[[#This Row],[吃饭]:[学习阅读]])</f>
-        <v>45</v>
+        <v>249.04000000000002</v>
       </c>
       <c r="N11" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>0</v>
+        <v>204.04000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>45637</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2.25</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -6004,19 +6025,23 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3">
         <f>SUM(表2_47891113[[#This Row],[吃饭]:[学习阅读]])</f>
-        <v>45</v>
+        <v>51.15</v>
       </c>
       <c r="N12" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>0</v>
+        <v>6.1499999999999986</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>45638</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="3">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3">
+        <v>9</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -6031,18 +6056,20 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3">
         <f>SUM(表2_47891113[[#This Row],[吃饭]:[学习阅读]])</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="N13" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>45639</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3">
+        <v>21.61</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -6055,26 +6082,33 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="3">
+        <v>27.1</v>
+      </c>
       <c r="M14" s="3">
         <f>SUM(表2_47891113[[#This Row],[吃饭]:[学习阅读]])</f>
-        <v>45</v>
+        <v>93.710000000000008</v>
       </c>
       <c r="N14" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>0</v>
+        <v>48.710000000000008</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>45640</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3">
+        <f>8.5+15</f>
+        <v>23.5</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3">
+        <v>40</v>
+      </c>
       <c r="H15" s="3">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -6085,11 +6119,11 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3">
         <f>SUM(表2_47891113[[#This Row],[吃饭]:[学习阅读]])</f>
-        <v>45</v>
+        <v>108.5</v>
       </c>
       <c r="N15" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>0</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -6557,15 +6591,15 @@
       </c>
       <c r="B33" s="3">
         <f>SUM(B2:B32)</f>
-        <v>263.70999999999998</v>
+        <v>553.95999999999992</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" ref="C33:I33" si="1">SUM(C2:C32)</f>
-        <v>0</v>
+        <v>26.45</v>
       </c>
       <c r="D33" s="3">
         <f>SUM(D2:D32)</f>
-        <v>398</v>
+        <v>532.24</v>
       </c>
       <c r="E33" s="3">
         <f t="shared" si="1"/>
@@ -6573,11 +6607,11 @@
       </c>
       <c r="F33" s="3">
         <f>SUM(F2:F32)</f>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="1"/>
-        <v>187.78</v>
+        <v>227.78</v>
       </c>
       <c r="H33" s="3">
         <f t="shared" si="1"/>
@@ -6597,15 +6631,15 @@
       </c>
       <c r="L33" s="3">
         <f>SUM(L2:L32)</f>
-        <v>0</v>
+        <v>27.1</v>
       </c>
       <c r="M33" s="5">
         <f>SUM(M2:M32)</f>
-        <v>2354.4899999999998</v>
+        <v>2881.5299999999997</v>
       </c>
       <c r="N33" s="3">
         <f>表2_47891113[[#This Row],[合计]]-表2_47891113[[#This Row],[房租]]-表2_47891113[[#This Row],[水电话费]]</f>
-        <v>859.48999999999978</v>
+        <v>1386.5299999999997</v>
       </c>
       <c r="P33" s="3"/>
     </row>
@@ -6622,14 +6656,14 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3">
         <f>SUM(B33:L33)</f>
-        <v>2354.4899999999998</v>
+        <v>2881.53</v>
       </c>
       <c r="M34" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N32">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7524,7 +7558,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N30">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8581,7 +8615,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N32">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9687,7 +9721,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10779,7 +10813,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N32">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11833,7 +11867,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12969,7 +13003,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N32">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14120,7 +14154,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N32">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15203,7 +15237,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>